<commit_message>
Patch Keypad VS Outlet productitemCreate
</commit_message>
<xml_diff>
--- a/excel/excelOrder99.xlsx
+++ b/excel/excelOrder99.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-112720" yWindow="-2740" windowWidth="25600" windowHeight="15620"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
-    <sheet name="Worksheet 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet 1" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>Contact</t>
   </si>
@@ -154,15 +150,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -173,30 +177,31 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -486,17 +491,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
@@ -508,20 +513,25 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="I2"/>
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="M2"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B3"/>
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I3"/>
       <c r="L3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="M3"/>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
@@ -533,6 +543,7 @@
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I4"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
@@ -541,6 +552,7 @@
       <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="I5"/>
       <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
@@ -552,6 +564,8 @@
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B6"/>
+      <c r="I6"/>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
@@ -601,6 +615,7 @@
       </c>
     </row>
     <row r="9" spans="1:15">
+      <c r="A9"/>
       <c r="B9" t="s">
         <v>30</v>
       </c>
@@ -616,6 +631,7 @@
       <c r="F9" t="s">
         <v>33</v>
       </c>
+      <c r="G9"/>
       <c r="H9" t="s">
         <v>34</v>
       </c>
@@ -642,6 +658,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
+      <c r="A10"/>
       <c r="B10" t="s">
         <v>36</v>
       </c>
@@ -686,6 +703,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
+      <c r="A11"/>
       <c r="B11" t="s">
         <v>40</v>
       </c>
@@ -730,30 +748,45 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>